<commit_message>
Code and necessary files added. All timing data collected
</commit_message>
<xml_diff>
--- a/CW2/Timing data.xlsx
+++ b/CW2/Timing data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Year 3\Intro-to-High-Performance-Conputing\CW2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D67C42-4102-4965-BF94-A44BA3E91C97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD7EBB9-4710-4CA1-9D3C-728F786E8707}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -444,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L117" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P139" sqref="P139"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB133" sqref="AB133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7109,14 +7109,24 @@
       <c r="W93">
         <v>2</v>
       </c>
-      <c r="X93" s="2"/>
-      <c r="Y93" s="2"/>
-      <c r="Z93" s="2"/>
-      <c r="AA93" s="2"/>
-      <c r="AB93" s="2"/>
+      <c r="X93" s="2">
+        <v>4.3E-3</v>
+      </c>
+      <c r="Y93" s="2">
+        <v>4.9760000000000004E-3</v>
+      </c>
+      <c r="Z93" s="2">
+        <v>4.3E-3</v>
+      </c>
+      <c r="AA93" s="2">
+        <v>4.3509999999999998E-3</v>
+      </c>
+      <c r="AB93" s="2">
+        <v>4.3140000000000001E-3</v>
+      </c>
       <c r="AC93" s="2">
         <f t="shared" ref="AC93:AC111" si="8">SUM(X93:AB93)/5</f>
-        <v>0</v>
+        <v>4.4481999999999994E-3</v>
       </c>
     </row>
     <row r="94" spans="2:29" x14ac:dyDescent="0.3">
@@ -7176,14 +7186,24 @@
       <c r="W94">
         <v>3</v>
       </c>
-      <c r="X94" s="2"/>
-      <c r="Y94" s="2"/>
-      <c r="Z94" s="2"/>
-      <c r="AA94" s="2"/>
-      <c r="AB94" s="2"/>
+      <c r="X94" s="2">
+        <v>5.4679999999999998E-3</v>
+      </c>
+      <c r="Y94" s="2">
+        <v>6.7010000000000004E-3</v>
+      </c>
+      <c r="Z94" s="2">
+        <v>6.4650000000000003E-3</v>
+      </c>
+      <c r="AA94" s="2">
+        <v>6.084E-3</v>
+      </c>
+      <c r="AB94" s="2">
+        <v>5.4510000000000001E-3</v>
+      </c>
       <c r="AC94" s="2">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>6.0337999999999998E-3</v>
       </c>
     </row>
     <row r="95" spans="2:29" x14ac:dyDescent="0.3">
@@ -7243,14 +7263,24 @@
       <c r="W95">
         <v>4</v>
       </c>
-      <c r="X95" s="2"/>
-      <c r="Y95" s="2"/>
-      <c r="Z95" s="2"/>
-      <c r="AA95" s="2"/>
-      <c r="AB95" s="2"/>
+      <c r="X95" s="2">
+        <v>6.881E-3</v>
+      </c>
+      <c r="Y95" s="2">
+        <v>6.0939999999999996E-3</v>
+      </c>
+      <c r="Z95" s="2">
+        <v>5.9069999999999999E-3</v>
+      </c>
+      <c r="AA95" s="2">
+        <v>6.9369999999999996E-3</v>
+      </c>
+      <c r="AB95" s="2">
+        <v>6.3049999999999998E-3</v>
+      </c>
       <c r="AC95" s="2">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>6.4247999999999996E-3</v>
       </c>
     </row>
     <row r="96" spans="2:29" x14ac:dyDescent="0.3">
@@ -7310,14 +7340,24 @@
       <c r="W96">
         <v>5</v>
       </c>
-      <c r="X96" s="2"/>
-      <c r="Y96" s="2"/>
-      <c r="Z96" s="2"/>
-      <c r="AA96" s="2"/>
-      <c r="AB96" s="2"/>
+      <c r="X96" s="2">
+        <v>5.6990000000000001E-3</v>
+      </c>
+      <c r="Y96" s="2">
+        <v>5.8040000000000001E-3</v>
+      </c>
+      <c r="Z96" s="2">
+        <v>5.6730000000000001E-3</v>
+      </c>
+      <c r="AA96" s="2">
+        <v>5.9100000000000003E-3</v>
+      </c>
+      <c r="AB96" s="2">
+        <v>4.463E-3</v>
+      </c>
       <c r="AC96" s="2">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>5.5098000000000005E-3</v>
       </c>
     </row>
     <row r="97" spans="2:29" x14ac:dyDescent="0.3">
@@ -7377,14 +7417,24 @@
       <c r="W97">
         <v>6</v>
       </c>
-      <c r="X97" s="2"/>
-      <c r="Y97" s="2"/>
-      <c r="Z97" s="2"/>
-      <c r="AA97" s="2"/>
-      <c r="AB97" s="2"/>
+      <c r="X97" s="2">
+        <v>6.3509999999999999E-3</v>
+      </c>
+      <c r="Y97" s="2">
+        <v>6.8950000000000001E-3</v>
+      </c>
+      <c r="Z97" s="2">
+        <v>6.9199999999999999E-3</v>
+      </c>
+      <c r="AA97" s="2">
+        <v>6.5189999999999996E-3</v>
+      </c>
+      <c r="AB97" s="2">
+        <v>5.9090000000000002E-3</v>
+      </c>
       <c r="AC97" s="2">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>6.5187999999999999E-3</v>
       </c>
     </row>
     <row r="98" spans="2:29" x14ac:dyDescent="0.3">
@@ -7444,14 +7494,24 @@
       <c r="W98">
         <v>7</v>
       </c>
-      <c r="X98" s="2"/>
-      <c r="Y98" s="2"/>
-      <c r="Z98" s="2"/>
-      <c r="AA98" s="2"/>
-      <c r="AB98" s="2"/>
+      <c r="X98" s="2">
+        <v>8.9990000000000001E-3</v>
+      </c>
+      <c r="Y98" s="2">
+        <v>4.607E-3</v>
+      </c>
+      <c r="Z98" s="2">
+        <v>5.522E-3</v>
+      </c>
+      <c r="AA98" s="2">
+        <v>7.2610000000000001E-3</v>
+      </c>
+      <c r="AB98" s="2">
+        <v>6.6119999999999998E-3</v>
+      </c>
       <c r="AC98" s="2">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>6.6002000000000005E-3</v>
       </c>
     </row>
     <row r="99" spans="2:29" x14ac:dyDescent="0.3">
@@ -7511,14 +7571,24 @@
       <c r="W99">
         <v>8</v>
       </c>
-      <c r="X99" s="2"/>
-      <c r="Y99" s="2"/>
-      <c r="Z99" s="2"/>
-      <c r="AA99" s="2"/>
-      <c r="AB99" s="2"/>
+      <c r="X99" s="2">
+        <v>4.4749999999999998E-3</v>
+      </c>
+      <c r="Y99" s="2">
+        <v>6.0280000000000004E-3</v>
+      </c>
+      <c r="Z99" s="2">
+        <v>6.215E-3</v>
+      </c>
+      <c r="AA99" s="2">
+        <v>6.5750000000000001E-3</v>
+      </c>
+      <c r="AB99" s="2">
+        <v>4.5269999999999998E-3</v>
+      </c>
       <c r="AC99" s="2">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>5.5640000000000004E-3</v>
       </c>
     </row>
     <row r="100" spans="2:29" x14ac:dyDescent="0.3">
@@ -7578,14 +7648,24 @@
       <c r="W100">
         <v>9</v>
       </c>
-      <c r="X100" s="2"/>
-      <c r="Y100" s="2"/>
-      <c r="Z100" s="2"/>
-      <c r="AA100" s="2"/>
-      <c r="AB100" s="2"/>
+      <c r="X100" s="2">
+        <v>0.10738</v>
+      </c>
+      <c r="Y100" s="2">
+        <v>7.5799999999999999E-3</v>
+      </c>
+      <c r="Z100" s="2">
+        <v>4.6090000000000002E-3</v>
+      </c>
+      <c r="AA100" s="2">
+        <v>9.5135999999999998E-2</v>
+      </c>
+      <c r="AB100" s="2">
+        <v>6.8278000000000005E-2</v>
+      </c>
       <c r="AC100" s="2">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>5.6596599999999997E-2</v>
       </c>
     </row>
     <row r="101" spans="2:29" x14ac:dyDescent="0.3">
@@ -7645,14 +7725,24 @@
       <c r="W101">
         <v>10</v>
       </c>
-      <c r="X101" s="2"/>
-      <c r="Y101" s="2"/>
-      <c r="Z101" s="2"/>
-      <c r="AA101" s="2"/>
-      <c r="AB101" s="2"/>
+      <c r="X101" s="2">
+        <v>8.7030000000000007E-3</v>
+      </c>
+      <c r="Y101" s="2">
+        <v>4.6179999999999997E-3</v>
+      </c>
+      <c r="Z101" s="2">
+        <v>4.4970000000000001E-3</v>
+      </c>
+      <c r="AA101" s="2">
+        <v>5.032E-3</v>
+      </c>
+      <c r="AB101" s="2">
+        <v>4.9880000000000002E-3</v>
+      </c>
       <c r="AC101" s="2">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>5.5676000000000007E-3</v>
       </c>
     </row>
     <row r="102" spans="2:29" x14ac:dyDescent="0.3">
@@ -7712,14 +7802,24 @@
       <c r="W102">
         <v>12</v>
       </c>
-      <c r="X102" s="2"/>
-      <c r="Y102" s="2"/>
-      <c r="Z102" s="2"/>
-      <c r="AA102" s="2"/>
-      <c r="AB102" s="2"/>
+      <c r="X102" s="2">
+        <v>6.8019999999999999E-3</v>
+      </c>
+      <c r="Y102" s="2">
+        <v>0.172598</v>
+      </c>
+      <c r="Z102" s="2">
+        <v>0.110495</v>
+      </c>
+      <c r="AA102" s="2">
+        <v>0.162693</v>
+      </c>
+      <c r="AB102" s="2">
+        <v>0.165802</v>
+      </c>
       <c r="AC102" s="2">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.123678</v>
       </c>
     </row>
     <row r="103" spans="2:29" x14ac:dyDescent="0.3">
@@ -7779,14 +7879,24 @@
       <c r="W103">
         <v>14</v>
       </c>
-      <c r="X103" s="2"/>
-      <c r="Y103" s="2"/>
-      <c r="Z103" s="2"/>
-      <c r="AA103" s="2"/>
-      <c r="AB103" s="2"/>
+      <c r="X103" s="2">
+        <v>0.27704000000000001</v>
+      </c>
+      <c r="Y103" s="2">
+        <v>0.12509799999999999</v>
+      </c>
+      <c r="Z103" s="2">
+        <v>9.9830000000000006E-3</v>
+      </c>
+      <c r="AA103" s="2">
+        <v>7.7640000000000001E-3</v>
+      </c>
+      <c r="AB103" s="2">
+        <v>6.6319999999999999E-3</v>
+      </c>
       <c r="AC103" s="2">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8.5303400000000001E-2</v>
       </c>
     </row>
     <row r="104" spans="2:29" x14ac:dyDescent="0.3">
@@ -7846,14 +7956,24 @@
       <c r="W104">
         <v>16</v>
       </c>
-      <c r="X104" s="2"/>
-      <c r="Y104" s="2"/>
-      <c r="Z104" s="2"/>
-      <c r="AA104" s="2"/>
-      <c r="AB104" s="2"/>
+      <c r="X104" s="2">
+        <v>0.27704000000000001</v>
+      </c>
+      <c r="Y104" s="2">
+        <v>0.12509799999999999</v>
+      </c>
+      <c r="Z104" s="2">
+        <v>9.9830000000000006E-3</v>
+      </c>
+      <c r="AA104" s="2">
+        <v>7.7640000000000001E-3</v>
+      </c>
+      <c r="AB104" s="2">
+        <v>6.6319999999999999E-3</v>
+      </c>
       <c r="AC104" s="2">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8.5303400000000001E-2</v>
       </c>
     </row>
     <row r="105" spans="2:29" x14ac:dyDescent="0.3">
@@ -7913,14 +8033,24 @@
       <c r="W105">
         <v>18</v>
       </c>
-      <c r="X105" s="2"/>
-      <c r="Y105" s="2"/>
-      <c r="Z105" s="2"/>
-      <c r="AA105" s="2"/>
-      <c r="AB105" s="2"/>
+      <c r="X105" s="2">
+        <v>0.177564</v>
+      </c>
+      <c r="Y105" s="2">
+        <v>0.24526800000000001</v>
+      </c>
+      <c r="Z105" s="2">
+        <v>0.206123</v>
+      </c>
+      <c r="AA105" s="2">
+        <v>0.29887200000000003</v>
+      </c>
+      <c r="AB105" s="2">
+        <v>0.41246100000000002</v>
+      </c>
       <c r="AC105" s="2">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.26805760000000001</v>
       </c>
     </row>
     <row r="106" spans="2:29" x14ac:dyDescent="0.3">
@@ -7980,14 +8110,24 @@
       <c r="W106">
         <v>20</v>
       </c>
-      <c r="X106" s="2"/>
-      <c r="Y106" s="2"/>
-      <c r="Z106" s="2"/>
-      <c r="AA106" s="2"/>
-      <c r="AB106" s="2"/>
+      <c r="X106" s="2">
+        <v>0.21778400000000001</v>
+      </c>
+      <c r="Y106" s="2">
+        <v>2.4847999999999999E-2</v>
+      </c>
+      <c r="Z106" s="2">
+        <v>1.0624E-2</v>
+      </c>
+      <c r="AA106" s="2">
+        <v>0.22184699999999999</v>
+      </c>
+      <c r="AB106" s="2">
+        <v>0.36779099999999998</v>
+      </c>
       <c r="AC106" s="2">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.1685788</v>
       </c>
     </row>
     <row r="107" spans="2:29" x14ac:dyDescent="0.3">
@@ -8047,14 +8187,24 @@
       <c r="W107">
         <v>22</v>
       </c>
-      <c r="X107" s="2"/>
-      <c r="Y107" s="2"/>
-      <c r="Z107" s="2"/>
-      <c r="AA107" s="2"/>
-      <c r="AB107" s="2"/>
+      <c r="X107" s="2">
+        <v>5.0848999999999998E-2</v>
+      </c>
+      <c r="Y107" s="2">
+        <v>0.26322499999999999</v>
+      </c>
+      <c r="Z107" s="2">
+        <v>0.18569099999999999</v>
+      </c>
+      <c r="AA107" s="2">
+        <v>0.23388800000000001</v>
+      </c>
+      <c r="AB107" s="2">
+        <v>0.20404800000000001</v>
+      </c>
       <c r="AC107" s="2">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.18754019999999999</v>
       </c>
     </row>
     <row r="108" spans="2:29" x14ac:dyDescent="0.3">
@@ -8114,14 +8264,24 @@
       <c r="W108">
         <v>24</v>
       </c>
-      <c r="X108" s="2"/>
-      <c r="Y108" s="2"/>
-      <c r="Z108" s="2"/>
-      <c r="AA108" s="2"/>
-      <c r="AB108" s="2"/>
+      <c r="X108" s="2">
+        <v>0.113939</v>
+      </c>
+      <c r="Y108" s="2">
+        <v>0.183503</v>
+      </c>
+      <c r="Z108" s="2">
+        <v>0.12995599999999999</v>
+      </c>
+      <c r="AA108" s="2">
+        <v>0.28311599999999998</v>
+      </c>
+      <c r="AB108" s="2">
+        <v>0.14461199999999999</v>
+      </c>
       <c r="AC108" s="2">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.17102519999999996</v>
       </c>
     </row>
     <row r="109" spans="2:29" x14ac:dyDescent="0.3">
@@ -8181,14 +8341,24 @@
       <c r="W109">
         <v>26</v>
       </c>
-      <c r="X109" s="2"/>
-      <c r="Y109" s="2"/>
-      <c r="Z109" s="2"/>
-      <c r="AA109" s="2"/>
-      <c r="AB109" s="2"/>
+      <c r="X109" s="2">
+        <v>0.47208</v>
+      </c>
+      <c r="Y109" s="2">
+        <v>0.13689299999999999</v>
+      </c>
+      <c r="Z109" s="2">
+        <v>6.9712999999999997E-2</v>
+      </c>
+      <c r="AA109" s="2">
+        <v>0.11792999999999999</v>
+      </c>
+      <c r="AB109" s="2">
+        <v>9.1983999999999996E-2</v>
+      </c>
       <c r="AC109" s="2">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.17771999999999999</v>
       </c>
     </row>
     <row r="110" spans="2:29" x14ac:dyDescent="0.3">
@@ -8248,14 +8418,24 @@
       <c r="W110">
         <v>28</v>
       </c>
-      <c r="X110" s="2"/>
-      <c r="Y110" s="2"/>
-      <c r="Z110" s="2"/>
-      <c r="AA110" s="2"/>
-      <c r="AB110" s="2"/>
+      <c r="X110" s="2">
+        <v>0.56765100000000002</v>
+      </c>
+      <c r="Y110" s="2">
+        <v>1.3899E-2</v>
+      </c>
+      <c r="Z110" s="2">
+        <v>1.2274E-2</v>
+      </c>
+      <c r="AA110" s="2">
+        <v>2.9822999999999999E-2</v>
+      </c>
+      <c r="AB110" s="2">
+        <v>1.4338999999999999E-2</v>
+      </c>
       <c r="AC110" s="2">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.12759720000000002</v>
       </c>
     </row>
     <row r="111" spans="2:29" x14ac:dyDescent="0.3">
@@ -8315,14 +8495,24 @@
       <c r="W111">
         <v>56</v>
       </c>
-      <c r="X111" s="2"/>
-      <c r="Y111" s="2"/>
-      <c r="Z111" s="2"/>
-      <c r="AA111" s="2"/>
-      <c r="AB111" s="2"/>
+      <c r="X111" s="2">
+        <v>0.62446299999999999</v>
+      </c>
+      <c r="Y111" s="2">
+        <v>4.7230000000000001E-2</v>
+      </c>
+      <c r="Z111" s="2">
+        <v>4.7632000000000001E-2</v>
+      </c>
+      <c r="AA111" s="2">
+        <v>0.10287300000000001</v>
+      </c>
+      <c r="AB111" s="2">
+        <v>2.3654000000000001E-2</v>
+      </c>
       <c r="AC111" s="2">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.1691704</v>
       </c>
     </row>
     <row r="113" spans="2:29" x14ac:dyDescent="0.3">
@@ -8470,14 +8660,24 @@
       <c r="W115">
         <v>2</v>
       </c>
-      <c r="X115" s="2"/>
-      <c r="Y115" s="2"/>
-      <c r="Z115" s="2"/>
-      <c r="AA115" s="2"/>
-      <c r="AB115" s="2"/>
+      <c r="X115" s="2">
+        <v>9.5589999999999998E-3</v>
+      </c>
+      <c r="Y115" s="2">
+        <v>1.1979999999999999E-2</v>
+      </c>
+      <c r="Z115" s="2">
+        <v>1.3820000000000001E-2</v>
+      </c>
+      <c r="AA115" s="2">
+        <v>1.7468999999999998E-2</v>
+      </c>
+      <c r="AB115" s="2">
+        <v>1.6319E-2</v>
+      </c>
       <c r="AC115" s="2">
         <f t="shared" ref="AC115:AC132" si="11">SUM(X115:AB115)/5</f>
-        <v>0</v>
+        <v>1.38294E-2</v>
       </c>
     </row>
     <row r="116" spans="2:29" x14ac:dyDescent="0.3">
@@ -8537,14 +8737,24 @@
       <c r="W116">
         <v>3</v>
       </c>
-      <c r="X116" s="2"/>
-      <c r="Y116" s="2"/>
-      <c r="Z116" s="2"/>
-      <c r="AA116" s="2"/>
-      <c r="AB116" s="2"/>
+      <c r="X116" s="2">
+        <v>2.1232999999999998E-2</v>
+      </c>
+      <c r="Y116" s="2">
+        <v>2.1315000000000001E-2</v>
+      </c>
+      <c r="Z116" s="2">
+        <v>1.0711999999999999E-2</v>
+      </c>
+      <c r="AA116" s="2">
+        <v>1.5858000000000001E-2</v>
+      </c>
+      <c r="AB116" s="2">
+        <v>2.4036999999999999E-2</v>
+      </c>
       <c r="AC116" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1.8631000000000002E-2</v>
       </c>
     </row>
     <row r="117" spans="2:29" x14ac:dyDescent="0.3">
@@ -8604,14 +8814,24 @@
       <c r="W117">
         <v>4</v>
       </c>
-      <c r="X117" s="2"/>
-      <c r="Y117" s="2"/>
-      <c r="Z117" s="2"/>
-      <c r="AA117" s="2"/>
-      <c r="AB117" s="2"/>
+      <c r="X117" s="2">
+        <v>2.649E-2</v>
+      </c>
+      <c r="Y117" s="2">
+        <v>1.3974E-2</v>
+      </c>
+      <c r="Z117" s="2">
+        <v>1.2239E-2</v>
+      </c>
+      <c r="AA117" s="2">
+        <v>1.2086E-2</v>
+      </c>
+      <c r="AB117" s="2">
+        <v>1.2194999999999999E-2</v>
+      </c>
       <c r="AC117" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1.5396799999999999E-2</v>
       </c>
     </row>
     <row r="118" spans="2:29" x14ac:dyDescent="0.3">
@@ -8671,14 +8891,24 @@
       <c r="W118">
         <v>5</v>
       </c>
-      <c r="X118" s="2"/>
-      <c r="Y118" s="2"/>
-      <c r="Z118" s="2"/>
-      <c r="AA118" s="2"/>
-      <c r="AB118" s="2"/>
+      <c r="X118" s="2">
+        <v>1.5247E-2</v>
+      </c>
+      <c r="Y118" s="2">
+        <v>2.7316E-2</v>
+      </c>
+      <c r="Z118" s="2">
+        <v>2.3779000000000002E-2</v>
+      </c>
+      <c r="AA118" s="2">
+        <v>1.5633000000000001E-2</v>
+      </c>
+      <c r="AB118" s="2">
+        <v>1.5491E-2</v>
+      </c>
       <c r="AC118" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1.9493200000000006E-2</v>
       </c>
     </row>
     <row r="119" spans="2:29" x14ac:dyDescent="0.3">
@@ -8738,14 +8968,24 @@
       <c r="W119">
         <v>6</v>
       </c>
-      <c r="X119" s="2"/>
-      <c r="Y119" s="2"/>
-      <c r="Z119" s="2"/>
-      <c r="AA119" s="2"/>
-      <c r="AB119" s="2"/>
+      <c r="X119" s="2">
+        <v>2.5208999999999999E-2</v>
+      </c>
+      <c r="Y119" s="2">
+        <v>3.9017999999999997E-2</v>
+      </c>
+      <c r="Z119" s="2">
+        <v>1.4037000000000001E-2</v>
+      </c>
+      <c r="AA119" s="2">
+        <v>3.0346999999999999E-2</v>
+      </c>
+      <c r="AB119" s="2">
+        <v>1.7994E-2</v>
+      </c>
       <c r="AC119" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>2.5321E-2</v>
       </c>
     </row>
     <row r="120" spans="2:29" x14ac:dyDescent="0.3">
@@ -8805,14 +9045,24 @@
       <c r="W120">
         <v>7</v>
       </c>
-      <c r="X120" s="2"/>
-      <c r="Y120" s="2"/>
-      <c r="Z120" s="2"/>
-      <c r="AA120" s="2"/>
-      <c r="AB120" s="2"/>
+      <c r="X120" s="2">
+        <v>4.7135999999999997E-2</v>
+      </c>
+      <c r="Y120" s="2">
+        <v>2.8195999999999999E-2</v>
+      </c>
+      <c r="Z120" s="2">
+        <v>2.5918E-2</v>
+      </c>
+      <c r="AA120" s="2">
+        <v>2.9340999999999999E-2</v>
+      </c>
+      <c r="AB120" s="2">
+        <v>2.9142000000000001E-2</v>
+      </c>
       <c r="AC120" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>3.1946599999999999E-2</v>
       </c>
     </row>
     <row r="121" spans="2:29" x14ac:dyDescent="0.3">
@@ -8872,14 +9122,24 @@
       <c r="W121">
         <v>8</v>
       </c>
-      <c r="X121" s="2"/>
-      <c r="Y121" s="2"/>
-      <c r="Z121" s="2"/>
-      <c r="AA121" s="2"/>
-      <c r="AB121" s="2"/>
+      <c r="X121" s="2">
+        <v>8.0348000000000003E-2</v>
+      </c>
+      <c r="Y121" s="2">
+        <v>2.8313999999999999E-2</v>
+      </c>
+      <c r="Z121" s="2">
+        <v>3.3370999999999998E-2</v>
+      </c>
+      <c r="AA121" s="2">
+        <v>3.2885999999999999E-2</v>
+      </c>
+      <c r="AB121" s="2">
+        <v>3.1556000000000001E-2</v>
+      </c>
       <c r="AC121" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>4.1295000000000005E-2</v>
       </c>
     </row>
     <row r="122" spans="2:29" x14ac:dyDescent="0.3">
@@ -8939,14 +9199,24 @@
       <c r="W122">
         <v>9</v>
       </c>
-      <c r="X122" s="2"/>
-      <c r="Y122" s="2"/>
-      <c r="Z122" s="2"/>
-      <c r="AA122" s="2"/>
-      <c r="AB122" s="2"/>
+      <c r="X122" s="2">
+        <v>1.8183000000000001E-2</v>
+      </c>
+      <c r="Y122" s="2">
+        <v>3.1674000000000001E-2</v>
+      </c>
+      <c r="Z122" s="2">
+        <v>2.5736999999999999E-2</v>
+      </c>
+      <c r="AA122" s="2">
+        <v>3.1261999999999998E-2</v>
+      </c>
+      <c r="AB122" s="2">
+        <v>3.1168999999999999E-2</v>
+      </c>
       <c r="AC122" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>2.7604999999999998E-2</v>
       </c>
     </row>
     <row r="123" spans="2:29" x14ac:dyDescent="0.3">
@@ -9006,14 +9276,24 @@
       <c r="W123">
         <v>10</v>
       </c>
-      <c r="X123" s="2"/>
-      <c r="Y123" s="2"/>
-      <c r="Z123" s="2"/>
-      <c r="AA123" s="2"/>
-      <c r="AB123" s="2"/>
+      <c r="X123" s="2">
+        <v>1.2538000000000001E-2</v>
+      </c>
+      <c r="Y123" s="2">
+        <v>1.3513000000000001E-2</v>
+      </c>
+      <c r="Z123" s="2">
+        <v>1.3903E-2</v>
+      </c>
+      <c r="AA123" s="2">
+        <v>2.0648E-2</v>
+      </c>
+      <c r="AB123" s="2">
+        <v>1.7177999999999999E-2</v>
+      </c>
       <c r="AC123" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1.5556E-2</v>
       </c>
     </row>
     <row r="124" spans="2:29" x14ac:dyDescent="0.3">
@@ -9073,14 +9353,24 @@
       <c r="W124">
         <v>12</v>
       </c>
-      <c r="X124" s="2"/>
-      <c r="Y124" s="2"/>
-      <c r="Z124" s="2"/>
-      <c r="AA124" s="2"/>
-      <c r="AB124" s="2"/>
+      <c r="X124" s="2">
+        <v>2.0282000000000001E-2</v>
+      </c>
+      <c r="Y124" s="2">
+        <v>1.3311E-2</v>
+      </c>
+      <c r="Z124" s="2">
+        <v>2.5440000000000001E-2</v>
+      </c>
+      <c r="AA124" s="2">
+        <v>2.8660999999999999E-2</v>
+      </c>
+      <c r="AB124" s="2">
+        <v>2.0795000000000001E-2</v>
+      </c>
       <c r="AC124" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>2.16978E-2</v>
       </c>
     </row>
     <row r="125" spans="2:29" x14ac:dyDescent="0.3">
@@ -9140,14 +9430,24 @@
       <c r="W125">
         <v>14</v>
       </c>
-      <c r="X125" s="2"/>
-      <c r="Y125" s="2"/>
-      <c r="Z125" s="2"/>
-      <c r="AA125" s="2"/>
-      <c r="AB125" s="2"/>
+      <c r="X125" s="2">
+        <v>3.3696999999999998E-2</v>
+      </c>
+      <c r="Y125" s="2">
+        <v>4.4817999999999997E-2</v>
+      </c>
+      <c r="Z125" s="2">
+        <v>1.3408E-2</v>
+      </c>
+      <c r="AA125" s="2">
+        <v>4.6197000000000002E-2</v>
+      </c>
+      <c r="AB125" s="2">
+        <v>1.8249999999999999E-2</v>
+      </c>
       <c r="AC125" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>3.1274000000000003E-2</v>
       </c>
     </row>
     <row r="126" spans="2:29" x14ac:dyDescent="0.3">
@@ -9207,14 +9507,24 @@
       <c r="W126">
         <v>16</v>
       </c>
-      <c r="X126" s="2"/>
-      <c r="Y126" s="2"/>
-      <c r="Z126" s="2"/>
-      <c r="AA126" s="2"/>
-      <c r="AB126" s="2"/>
+      <c r="X126" s="2">
+        <v>7.9344999999999999E-2</v>
+      </c>
+      <c r="Y126" s="2">
+        <v>1.3127E-2</v>
+      </c>
+      <c r="Z126" s="2">
+        <v>5.151E-2</v>
+      </c>
+      <c r="AA126" s="2">
+        <v>5.9158000000000002E-2</v>
+      </c>
+      <c r="AB126" s="2">
+        <v>1.4533000000000001E-2</v>
+      </c>
       <c r="AC126" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>4.3534599999999993E-2</v>
       </c>
     </row>
     <row r="127" spans="2:29" x14ac:dyDescent="0.3">
@@ -9274,14 +9584,24 @@
       <c r="W127">
         <v>18</v>
       </c>
-      <c r="X127" s="2"/>
-      <c r="Y127" s="2"/>
-      <c r="Z127" s="2"/>
-      <c r="AA127" s="2"/>
-      <c r="AB127" s="2"/>
+      <c r="X127" s="2">
+        <v>1.8109E-2</v>
+      </c>
+      <c r="Y127" s="2">
+        <v>3.8924E-2</v>
+      </c>
+      <c r="Z127" s="2">
+        <v>3.7435000000000003E-2</v>
+      </c>
+      <c r="AA127" s="2">
+        <v>1.1638000000000001E-2</v>
+      </c>
+      <c r="AB127" s="2">
+        <v>5.0946999999999999E-2</v>
+      </c>
       <c r="AC127" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>3.1410599999999997E-2</v>
       </c>
     </row>
     <row r="128" spans="2:29" x14ac:dyDescent="0.3">
@@ -9341,14 +9661,24 @@
       <c r="W128">
         <v>20</v>
       </c>
-      <c r="X128" s="2"/>
-      <c r="Y128" s="2"/>
-      <c r="Z128" s="2"/>
-      <c r="AA128" s="2"/>
-      <c r="AB128" s="2"/>
+      <c r="X128" s="2">
+        <v>1.3358E-2</v>
+      </c>
+      <c r="Y128" s="2">
+        <v>1.3207999999999999E-2</v>
+      </c>
+      <c r="Z128" s="2">
+        <v>7.8900999999999999E-2</v>
+      </c>
+      <c r="AA128" s="2">
+        <v>8.9417999999999997E-2</v>
+      </c>
+      <c r="AB128" s="2">
+        <v>0.12805</v>
+      </c>
       <c r="AC128" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>6.4586999999999992E-2</v>
       </c>
     </row>
     <row r="129" spans="2:31" x14ac:dyDescent="0.3">
@@ -9408,14 +9738,24 @@
       <c r="W129">
         <v>22</v>
       </c>
-      <c r="X129" s="2"/>
-      <c r="Y129" s="2"/>
-      <c r="Z129" s="2"/>
-      <c r="AA129" s="2"/>
-      <c r="AB129" s="2"/>
+      <c r="X129" s="2">
+        <v>2.7536000000000001E-2</v>
+      </c>
+      <c r="Y129" s="2">
+        <v>1.2418E-2</v>
+      </c>
+      <c r="Z129" s="2">
+        <v>0.10438</v>
+      </c>
+      <c r="AA129" s="2">
+        <v>3.0084E-2</v>
+      </c>
+      <c r="AB129" s="2">
+        <v>2.0989000000000001E-2</v>
+      </c>
       <c r="AC129" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>3.9081400000000002E-2</v>
       </c>
     </row>
     <row r="130" spans="2:31" x14ac:dyDescent="0.3">
@@ -9475,14 +9815,24 @@
       <c r="W130">
         <v>24</v>
       </c>
-      <c r="X130" s="2"/>
-      <c r="Y130" s="2"/>
-      <c r="Z130" s="2"/>
-      <c r="AA130" s="2"/>
-      <c r="AB130" s="2"/>
+      <c r="X130" s="2">
+        <v>0.19158600000000001</v>
+      </c>
+      <c r="Y130" s="2">
+        <v>0.15037800000000001</v>
+      </c>
+      <c r="Z130" s="2">
+        <v>0.150231</v>
+      </c>
+      <c r="AA130" s="2">
+        <v>0.12665799999999999</v>
+      </c>
+      <c r="AB130" s="2">
+        <v>0.13945099999999999</v>
+      </c>
       <c r="AC130" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.15166080000000001</v>
       </c>
     </row>
     <row r="131" spans="2:31" x14ac:dyDescent="0.3">
@@ -9542,14 +9892,24 @@
       <c r="W131">
         <v>26</v>
       </c>
-      <c r="X131" s="2"/>
-      <c r="Y131" s="2"/>
-      <c r="Z131" s="2"/>
-      <c r="AA131" s="2"/>
-      <c r="AB131" s="2"/>
+      <c r="X131" s="2">
+        <v>0.10864500000000001</v>
+      </c>
+      <c r="Y131" s="2">
+        <v>0.170991</v>
+      </c>
+      <c r="Z131" s="2">
+        <v>0.131216</v>
+      </c>
+      <c r="AA131" s="2">
+        <v>0.17532500000000001</v>
+      </c>
+      <c r="AB131" s="2">
+        <v>0.186806</v>
+      </c>
       <c r="AC131" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.1545966</v>
       </c>
     </row>
     <row r="132" spans="2:31" x14ac:dyDescent="0.3">
@@ -9609,14 +9969,24 @@
       <c r="W132">
         <v>28</v>
       </c>
-      <c r="X132" s="2"/>
-      <c r="Y132" s="2"/>
-      <c r="Z132" s="2"/>
-      <c r="AA132" s="2"/>
-      <c r="AB132" s="2"/>
+      <c r="X132" s="2">
+        <v>0.18029800000000001</v>
+      </c>
+      <c r="Y132" s="2">
+        <v>0.24496100000000001</v>
+      </c>
+      <c r="Z132" s="2">
+        <v>0.15149899999999999</v>
+      </c>
+      <c r="AA132" s="2">
+        <v>0.147511</v>
+      </c>
+      <c r="AB132" s="2">
+        <v>0.238089</v>
+      </c>
       <c r="AC132" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.19247160000000002</v>
       </c>
     </row>
     <row r="134" spans="2:31" x14ac:dyDescent="0.3">

</xml_diff>